<commit_message>
opis firmy littefuse oraz serii bezpieczników
</commit_message>
<xml_diff>
--- a/Littetlfuse/Littelfuse_grad.xlsx
+++ b/Littetlfuse/Littelfuse_grad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\microczp_notatki\zlecenie\Littetlfuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754EC546-F216-4F68-AFC1-D25B91FF3F02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60898BD9-DE6A-4DF9-8C22-D1D97338F5ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>W naszej ofercie znajdują się bezpieczniki specjalnego zastosowania renomowanej firmy Littelfuse, która jest światowym producentem wiodących technologi w zakresie ochorny obwodów, m.in. poprzez produkcję wyspecjalizowanych bezpieczników. Produktów tej firmy używa ponad 100 tysięcy klientów końcowych, a spotkać je można na każdym kroku m. in. w samochodach, sprzęcie medycznym, liniach produkcyjncyh, urządzeniach telekomunikacyjnych oraz codziennego użytku na całym świecie.</t>
+    <t xml:space="preserve">W naszej ofercie znajdują się bezpieczniki specjalnego zastosowania renomowanej firmy Littelfuse, która jest światowym producentem wiodących technologi w zakresie ochorny obwodów. Produktów tej firmy używa ponad 100 tysięcy klientów końcowych, a spotkać je można na każdym kroku m. in. w samochodach, sprzęcie medycznym, liniach produkcyjncyh, urządzeniach telekomunikacyjnych oraz sprzęcie codziennego użytku na całym świecie.
+Bezpieczniki serii 259 (0259.062T, 0259.125T, 0259.250T, 0259.375T) są przeznaczone do zastosowań w strefach niebezpiecznych, oraz zagrożonych wybuchem. Zostały one pierwotnie stworzone z myślą o potrzebach firm gazowniczych i przemysłu petrochemicznego, dlatego bezpieczniki są certyfikowane do użytku w urządzeniach iskrobezpiecznych z certyfikatami ATEX i IECEx dla prądów od 0.062A do 5A. 
+Bezpieczniki seri 251 (0251015.HAT1L) zostały zaprojektowane do zastosowań w urządzeniach gdzie krytycznym parametrem jest ich czas zadziałąnia. Są to bardzo szybko działające bezpieczniki chrakteryzujące się małym rozmiarem i szerokim zakresem temperatur i prądów pracy. 
+Bezpieczniki seri RXEF (RXEF250) charakteryzuje bardzo niski prąd podtrzymania (do 50 mA) oraz wysokie napięcie znamieniowe (do 72 V). </t>
   </si>
 </sst>
 </file>
@@ -348,15 +351,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="168" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="222" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -370,10 +373,12 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>